<commit_message>
light return to leetcode, wrote out / designed structure and approach
</commit_message>
<xml_diff>
--- a/Find Duplicate File in System/Whiteboards/Solution.xlsx
+++ b/Find Duplicate File in System/Whiteboards/Solution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Longest Palindromic Substring\Whiteboards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portalz\Desktop\Small Projects\LeetCode\Find Duplicate File in System\Whiteboards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DFE340-9EA5-43EC-9B8B-09BBE60FCC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53439325-736E-43FA-98CD-C4D00062DE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{756CC0B2-6BE7-4EF6-9EEE-182F71A93026}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>root/a</t>
+  </si>
+  <si>
+    <t>root/c</t>
+  </si>
+  <si>
+    <t>root/c/d</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -384,17 +404,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79CF585D-CE06-44D4-80AA-070156E711E0}">
-  <dimension ref="A1"/>
+  <dimension ref="F5:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="4.7109375" style="1"/>
+    <col min="1" max="9" width="4.7109375" style="1"/>
+    <col min="10" max="10" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="4.7109375" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="5" spans="6:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="6:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="6:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="6:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="6:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>3</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>